<commit_message>
commiting changes in excel and keyword engine
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/gap/testScenarios/keywords.xlsx
+++ b/src/main/java/com/qa/gap/testScenarios/keywords.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>TestStep</t>
   </si>
@@ -600,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,10 +994,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>16</v>
@@ -1007,16 +1007,44 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commiting changes for excel file and keyword engine
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/gap/testScenarios/keywords.xlsx
+++ b/src/main/java/com/qa/gap/testScenarios/keywords.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>TestStep</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>xpath:- //td[@class='xY a4W']//div[@class='xT']//span[@class='y2']</t>
+  </si>
+  <si>
+    <t>Enter email address.</t>
   </si>
 </sst>
 </file>
@@ -602,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +661,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
commiting changes for extent reports
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/gap/testScenarios/keywords.xlsx
+++ b/src/main/java/com/qa/gap/testScenarios/keywords.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="63">
   <si>
     <t>TestStep</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Verify successful login of user</t>
-  </si>
-  <si>
-    <t>xpath= //a[@title='Inbox']</t>
   </si>
   <si>
     <t>Click on Compose Button</t>
@@ -143,9 +140,6 @@
     <t>getText</t>
   </si>
   <si>
-    <t>Click on inbox Button</t>
-  </si>
-  <si>
     <t>Verify message</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
   </si>
   <si>
     <t>xpath:- //td[@class='xY a4W']//div[@class='xT']//span[@class='y2']</t>
-  </si>
-  <si>
-    <t>Enter email address.</t>
   </si>
 </sst>
 </file>
@@ -603,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +630,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -661,10 +652,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -678,7 +669,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -692,7 +683,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -706,7 +697,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -720,10 +711,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
@@ -731,10 +722,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -745,80 +736,80 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -829,10 +820,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>16</v>
@@ -843,13 +834,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>5</v>
@@ -863,10 +854,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,13 +879,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>16</v>
@@ -916,13 +907,13 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,7 +921,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>16</v>
@@ -944,10 +935,10 @@
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>5</v>
@@ -955,13 +946,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>5</v>
@@ -969,13 +960,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>5</v>
@@ -983,24 +974,24 @@
     </row>
     <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>16</v>
@@ -1011,10 +1002,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>16</v>
@@ -1024,30 +1015,16 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>41</v>
+      <c r="A30" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1076,10 +1053,10 @@
   <sheetData>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>

</xml_diff>